<commit_message>
Atualização da Planilha dos Entregaveis e da Qualidade dos entregaveis
</commit_message>
<xml_diff>
--- a/entregaveis.xlsx
+++ b/entregaveis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\'\Desktop\TCC\trunk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kokmz\Desktop\TCC\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Entregáveis" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entregáveis!$A$1:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entregáveis!#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Entregáveis</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Data prevista para conclusão</t>
   </si>
   <si>
-    <t>Modulo Documentação do histórico dos pacientes</t>
-  </si>
-  <si>
     <t>Modulo Geração prontuário digital para o paciente</t>
   </si>
   <si>
@@ -45,6 +42,12 @@
   </si>
   <si>
     <t>Situação dos entregáveis</t>
+  </si>
+  <si>
+    <t>Data da conclusão</t>
+  </si>
+  <si>
+    <t>Modulo Relatório do histórico de exames dos pacientes</t>
   </si>
 </sst>
 </file>
@@ -161,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -273,7 +276,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -423,83 +426,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="44.42578125" style="3"/>
+    <col min="4" max="4" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="44.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4">
         <v>42103</v>
       </c>
-      <c r="C2" s="6">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C2" s="4">
+        <v>42103</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4">
         <v>42110</v>
       </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C3" s="4">
+        <v>42114</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>42128</v>
       </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="4">
+        <v>42128</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
     </row>
   </sheetData>

</xml_diff>